<commit_message>
Committed on 05 may 2020
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/HolidayListData.xlsx
+++ b/ocms/src/test/resources/TestData/HolidayListData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\scripts\ocms\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADBB987-50CF-4005-B559-293EDEF3E667}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18720" windowHeight="8040"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -120,18 +121,30 @@
     <t>Scenarios</t>
   </si>
   <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>50001</t>
+  </si>
+  <si>
+    <t>19/12/2020</t>
+  </si>
+  <si>
+    <t>20/12/2020</t>
+  </si>
+  <si>
+    <t>12/11/2020</t>
+  </si>
+  <si>
+    <t>15/11/2020</t>
+  </si>
+  <si>
+    <t>21/12/2020</t>
+  </si>
+  <si>
     <t>22/12/2020</t>
   </si>
   <si>
-    <t>19/12/2020</t>
-  </si>
-  <si>
-    <t>20/12/2020</t>
-  </si>
-  <si>
-    <t>21/12/2020</t>
-  </si>
-  <si>
     <t>16/12/2020</t>
   </si>
   <si>
@@ -142,24 +155,12 @@
   </si>
   <si>
     <t>12/12/2020</t>
-  </si>
-  <si>
-    <t>12/11/2020</t>
-  </si>
-  <si>
-    <t>15/11/2020</t>
-  </si>
-  <si>
-    <t>50000</t>
-  </si>
-  <si>
-    <t>50001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -290,6 +291,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -325,6 +343,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,25 +535,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="7" max="7" width="33.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,18 +576,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -564,18 +599,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
@@ -587,18 +622,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>7</v>
@@ -610,18 +645,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>7</v>
@@ -633,18 +668,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
@@ -656,18 +691,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
@@ -679,18 +714,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>7</v>
@@ -708,25 +743,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="7" max="7" width="27.453125" customWidth="1"/>
+    <col min="8" max="8" width="26.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,18 +787,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -784,23 +819,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="30.54296875" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -826,18 +861,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -858,24 +893,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="83.85546875" customWidth="1"/>
+    <col min="1" max="1" width="83.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>